<commit_message>
Updated code for creating png files
</commit_message>
<xml_diff>
--- a/data/impacts/Impacts_labels.xlsx
+++ b/data/impacts/Impacts_labels.xlsx
@@ -441,98 +441,98 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Land Use (m2) Arable</t>
+          <t>Land Use Arable</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Land Use (m2) Fallow</t>
+          <t>Land Use Fallow</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Land Use (m2) Perm Past</t>
+          <t>Land Use Perm Past</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) LUC</t>
+          <t>GHG LUC</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Feed</t>
+          <t>GHG Feed</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Farm</t>
+          <t>GHG Farm</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Processing</t>
+          <t>GHG Processing</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Transport</t>
+          <t>GHG Transport</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Packging</t>
+          <t>GHG Packging</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Retail</t>
+          <t>GHG Retail</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Acid.(kg SO2eq)</t>
+          <t>Acidification</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Eutr. (kg PO43-eq)</t>
+          <t>Eutrophication</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Freshwater (L)</t>
+          <t>Freshwater Withdrawals (FW)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Str-Wt WU (L eq)</t>
+          <t>Scarcity-Weighted FW</t>
         </is>
       </c>
     </row>

</xml_diff>